<commit_message>
Adding README.md file for How To USE & File Path fix in Excel And Properties class
</commit_message>
<xml_diff>
--- a/TestData/Naukri_Automation_Details.xlsx
+++ b/TestData/Naukri_Automation_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practice_workspace\NaukriTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94532AA4-1CA1-4BDF-A6F5-E85E2C78FEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76433BD8-C2BE-415B-AE1F-531D1C324C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{736153B1-179A-4D3F-BA43-3150E3D1578F}"/>
   </bookViews>
@@ -51,19 +51,19 @@
     <t>applications</t>
   </si>
   <si>
-    <t>Mumbai, Navi Mumbai</t>
-  </si>
-  <si>
     <t>experience</t>
   </si>
   <si>
-    <t>demo123@gmail.com</t>
-  </si>
-  <si>
-    <t>demoPass@1234</t>
-  </si>
-  <si>
     <t xml:space="preserve">Automation Test Engineer, Java, Selenium </t>
+  </si>
+  <si>
+    <t>Mumbai, Navi Mumbai, pune</t>
+  </si>
+  <si>
+    <t>DemoPass@123</t>
+  </si>
+  <si>
+    <t>DemoEmail.gamil.com</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,32 +498,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
+    <hyperlink ref="A2" r:id="rId1" display="siddhesh.vedre12@gmail.com" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{E1B5ED84-FA52-4D95-A07F-3BCC4B578110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Excel Utility Bug Fix
</commit_message>
<xml_diff>
--- a/TestData/Naukri_Automation_Details.xlsx
+++ b/TestData/Naukri_Automation_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practice_workspace\NaukriTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76433BD8-C2BE-415B-AE1F-531D1C324C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50255A35-35B0-484C-B0C4-BE50CB4FBB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{736153B1-179A-4D3F-BA43-3150E3D1578F}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>DemoPass@123</t>
   </si>
   <si>
-    <t>DemoEmail.gamil.com</t>
+    <t>DemoLogin@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +476,7 @@
     <col min="1" max="1" width="25.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="41" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" style="4" customWidth="1"/>
   </cols>
@@ -518,12 +518,12 @@
         <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="siddhesh.vedre12@gmail.com" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{E1B5ED84-FA52-4D95-A07F-3BCC4B578110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding Project To JENKINS
</commit_message>
<xml_diff>
--- a/TestData/Naukri_Automation_Details.xlsx
+++ b/TestData/Naukri_Automation_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practice_workspace\NaukriTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50255A35-35B0-484C-B0C4-BE50CB4FBB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D77C7F-2E09-4F3A-AB18-89498E4325D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{736153B1-179A-4D3F-BA43-3150E3D1578F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -60,10 +60,13 @@
     <t>Mumbai, Navi Mumbai, pune</t>
   </si>
   <si>
-    <t>DemoPass@123</t>
-  </si>
-  <si>
-    <t>DemoLogin@gmail.com</t>
+    <t>siddhesh.vedre12@gmail.com</t>
+  </si>
+  <si>
+    <t>Mumbai, Navi Mumbai</t>
+  </si>
+  <si>
+    <t>naukri@Test123</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3108B3EC-137C-40B9-913D-5AB0E536CB8A}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,10 +506,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -515,9 +518,29 @@
         <v>7</v>
       </c>
       <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
         <v>3</v>
       </c>
     </row>
@@ -525,6 +548,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{E1B5ED84-FA52-4D95-A07F-3BCC4B578110}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{F434A67A-EE33-4C14-9F4C-43F42833C879}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{9BC9A4E5-8C6A-4E94-845E-0720320104C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Selenium Grid in Project
</commit_message>
<xml_diff>
--- a/TestData/Naukri_Automation_Details.xlsx
+++ b/TestData/Naukri_Automation_Details.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practice_workspace\NaukriTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D77C7F-2E09-4F3A-AB18-89498E4325D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FA45DC-6054-4FF2-BF97-75DE90645082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{736153B1-179A-4D3F-BA43-3150E3D1578F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -66,7 +67,40 @@
     <t>Mumbai, Navi Mumbai</t>
   </si>
   <si>
-    <t>naukri@Test123</t>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Test Result</t>
+  </si>
+  <si>
+    <t>Actual Test Result</t>
+  </si>
+  <si>
+    <t>Status Pass/Fail</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>TC001_JobSearchTest</t>
+  </si>
+  <si>
+    <t>TC002_ProfileUpdateDaily</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -111,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -134,12 +168,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,12 +298,234 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="medium">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -169,6 +536,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D609F932-7BCE-4DF8-B623-8EAD7CC274A4}" name="Table2" displayName="Table2" ref="A1:I5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I5" xr:uid="{D609F932-7BCE-4DF8-B623-8EAD7CC274A4}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{1FD9D90A-C138-4DB9-982D-25E730DB1C90}" name="Test Case ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1026A3B8-7060-4BB0-9531-2215E49FBF3A}" name="Test Case Description" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9589B2BE-B235-4D95-B1C2-A4A714B59F73}" name="Test Data" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{BB2E4F7C-80A1-46B8-8609-15968480F3A8}" name="Pre-Condition" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F15C3AC3-63A4-4032-B9A8-706122813A48}" name="Test Steps" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9D17B57E-53BC-4552-B871-355BA5FAE6A7}" name="Expected Test Result" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{36B091D5-E760-43EF-949D-57A9B88AB458}" name="Actual Test Result" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D2720CE4-B897-4B9C-904E-E7B90040E9DE}" name="Status Pass/Fail" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{E54FABA0-0352-42B3-AA83-965685708540}" name="Comments" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,7 +856,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +894,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -518,10 +903,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -529,7 +914,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -538,19 +923,126 @@
         <v>9</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{06891BE8-B6E0-44B5-8D89-98D1109A65C9}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{E1B5ED84-FA52-4D95-A07F-3BCC4B578110}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{F434A67A-EE33-4C14-9F4C-43F42833C879}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{9BC9A4E5-8C6A-4E94-845E-0720320104C0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F434A67A-EE33-4C14-9F4C-43F42833C879}"/>
+    <hyperlink ref="B2" r:id="rId3" display="automate@Sid123#" xr:uid="{E1B5ED84-FA52-4D95-A07F-3BCC4B578110}"/>
+    <hyperlink ref="B3" r:id="rId4" display="automate@Sid123#" xr:uid="{61F7F640-0A45-4B38-BD5E-7D9E52D5942A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFA0C57-B3D7-4B2C-8F1A-EE6EB4D24412}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="82.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>